<commit_message>
empece el fron-end hice comentes ectro esto y seteo de varuiables
</commit_message>
<xml_diff>
--- a/ServicioColasTP4.xlsx
+++ b/ServicioColasTP4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FACULTAD\Simulacion\TPS\TP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5B8B2C-A7FA-4BD3-B74D-3AF81919D4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57D7599-51EF-476B-9769-22B2641366FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{94BAB2D5-E658-40C1-BAF5-D15E57F44FB0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>Reloj</t>
   </si>
@@ -298,7 +298,31 @@
     <t>tpo. Variabl</t>
   </si>
   <si>
-    <t>Estado Servidores</t>
+    <t xml:space="preserve">Inicial </t>
+  </si>
+  <si>
+    <t>LlegadaCLiente TS4</t>
+  </si>
+  <si>
+    <t>fin aten TS4 C1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Servidores estados</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>….</t>
   </si>
 </sst>
 </file>
@@ -327,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +361,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -365,11 +431,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -377,7 +441,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D162BF1-DD64-42C2-A21E-E32E4504EB86}">
-  <dimension ref="B2:AM33"/>
+  <dimension ref="B2:AR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P7" workbookViewId="0">
-      <selection activeCell="AM22" sqref="AM22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,46 +806,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="6"/>
       <c r="D6">
         <v>3</v>
       </c>
@@ -791,10 +867,10 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="6"/>
       <c r="D7">
         <v>2</v>
       </c>
@@ -813,10 +889,10 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="6"/>
       <c r="D8">
         <v>3</v>
       </c>
@@ -829,10 +905,10 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="6"/>
       <c r="D9">
         <v>2</v>
       </c>
@@ -874,47 +950,51 @@
         <v>45</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="6"/>
       <c r="D14">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="6"/>
       <c r="D15">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="6"/>
       <c r="D16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="F16">
+        <f ca="1">RAND()</f>
+        <v>0.17828291981978617</v>
+      </c>
+    </row>
+    <row r="17" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
       <c r="D17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>41</v>
       </c>
@@ -923,34 +1003,47 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="AM21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="D22" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G22" t="s">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="J22" t="s">
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="M22" t="s">
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P22" t="s">
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="S22" s="5" t="s">
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="14"/>
       <c r="X22" t="s">
         <v>72</v>
       </c>
@@ -967,59 +1060,65 @@
         <v>77</v>
       </c>
       <c r="AM22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="13" t="s">
         <v>58</v>
       </c>
       <c r="S23" t="s">
@@ -1081,6 +1180,210 @@
       </c>
       <c r="AL23" t="s">
         <v>73</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.73</v>
+      </c>
+      <c r="E24">
+        <f>-25*LN(1-D24)</f>
+        <v>32.733332999594055</v>
+      </c>
+      <c r="F24">
+        <f>E24+C24</f>
+        <v>32.733332999594055</v>
+      </c>
+      <c r="G24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H24">
+        <f>-D15*LN(1-G24)</f>
+        <v>5.1373546342016398</v>
+      </c>
+      <c r="I24">
+        <f>H24+C24</f>
+        <v>5.1373546342016398</v>
+      </c>
+      <c r="J24">
+        <v>0.69</v>
+      </c>
+      <c r="K24">
+        <f>-30*LN(1-J24)</f>
+        <v>35.135489445088346</v>
+      </c>
+      <c r="L24">
+        <f>K24+C24</f>
+        <v>35.135489445088346</v>
+      </c>
+      <c r="M24">
+        <v>0.3</v>
+      </c>
+      <c r="N24">
+        <f>-$D$17*LN(1-M24)</f>
+        <v>3.5667494393873245</v>
+      </c>
+      <c r="O24" s="15">
+        <f>N24+C24</f>
+        <v>3.5667494393873245</v>
+      </c>
+      <c r="P24">
+        <v>0.94</v>
+      </c>
+      <c r="Q24">
+        <f>-8*LN(1-P24)</f>
+        <v>22.507285734080284</v>
+      </c>
+      <c r="R24">
+        <f>Q24+C24</f>
+        <v>22.507285734080284</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <v>0</v>
+      </c>
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24">
+        <v>0</v>
+      </c>
+      <c r="AK24">
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>0</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN24" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO24" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25">
+        <v>3.56</v>
+      </c>
+      <c r="F25">
+        <f>F24</f>
+        <v>32.733332999594055</v>
+      </c>
+      <c r="I25">
+        <f>I24</f>
+        <v>5.1373546342016398</v>
+      </c>
+      <c r="L25">
+        <f>L24</f>
+        <v>35.135489445088346</v>
+      </c>
+      <c r="M25">
+        <v>0.75</v>
+      </c>
+      <c r="N25">
+        <f>-$D$17*LN(1-M25)</f>
+        <v>13.862943611198906</v>
+      </c>
+      <c r="O25" s="16">
+        <f>N25+C25</f>
+        <v>17.422943611198907</v>
+      </c>
+      <c r="R25">
+        <f>R24</f>
+        <v>22.507285734080284</v>
+      </c>
+      <c r="AG25" s="17">
+        <f>0.2+C25</f>
+        <v>3.7600000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26">
+        <v>3.76</v>
+      </c>
+      <c r="O26">
+        <f>O25</f>
+        <v>17.422943611198907</v>
       </c>
     </row>
     <row r="33" spans="7:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,11 +1392,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="S22:W22"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -1103,6 +1401,11 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="S22:W22"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1209,10 +1512,10 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="6"/>
       <c r="G17" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>